<commit_message>
add steps for selecting category and prirority in create company
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/CompanyManagement.xlsx
+++ b/src/test/resources/DataFiles/CompanyManagement.xlsx
@@ -24,13 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
-  <si>
-    <t>USER_NAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>STATUS</t>
   </si>
@@ -41,21 +35,12 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>TestEmp123</t>
-  </si>
-  <si>
-    <t>Test@1234</t>
-  </si>
-  <si>
     <t>TC_ID</t>
   </si>
   <si>
     <t>TestEmp124</t>
   </si>
   <si>
-    <t>Test@1235</t>
-  </si>
-  <si>
     <t>76342434</t>
   </si>
   <si>
@@ -98,9 +83,6 @@
     <t>USERS_ACCESS</t>
   </si>
   <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
     <t>TestCompany</t>
   </si>
   <si>
@@ -108,24 +90,28 @@
   </si>
   <si>
     <t>New</t>
+  </si>
+  <si>
+    <t>PRIORITY</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>Partner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,17 +134,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,143 +434,126 @@
     <col min="5" max="5" width="21.08984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.90625" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2" display="Test@1234"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>